<commit_message>
Enhance NIP lookup strategies in BraveSearchService with email domain support; update requirements to include zeep for GUS API; normalize Polish characters in ZohoSearchService for improved matching; refine data normalization logic to validate NIP against email domains; delete temporary Excel files.
</commit_message>
<xml_diff>
--- a/test_comparison_report.xlsx
+++ b/test_comparison_report.xlsx
@@ -529,10 +529,10 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="n">
         <v>6</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>8</v>
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
@@ -565,10 +565,10 @@
         </is>
       </c>
       <c r="B9" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="n">
         <v>9</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>7</v>
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
@@ -583,10 +583,10 @@
         </is>
       </c>
       <c r="B10" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4" t="n">
         <v>9</v>
-      </c>
-      <c r="C10" s="4" t="n">
-        <v>7</v>
       </c>
       <c r="D10" s="4" t="inlineStr">
         <is>
@@ -636,15 +636,15 @@
           <t>Sygnaly E</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n">
-        <v>8</v>
+      <c r="B13" s="4" t="n">
+        <v>9</v>
       </c>
       <c r="C13" s="4" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D13" s="4" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>REMIS</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
         </is>
       </c>
       <c r="B14" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>0</v>
@@ -672,15 +672,15 @@
           <t>Sygnaly L</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n">
-        <v>10</v>
+      <c r="B15" s="4" t="n">
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D15" s="4" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>REMIS</t>
         </is>
       </c>
     </row>
@@ -690,15 +690,15 @@
           <t>Sygnaly F</t>
         </is>
       </c>
-      <c r="B16" s="5" t="n">
-        <v>10</v>
+      <c r="B16" s="4" t="n">
+        <v>11</v>
       </c>
       <c r="C16" s="4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D16" s="4" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>REMIS</t>
         </is>
       </c>
     </row>
@@ -774,14 +774,14 @@
         </is>
       </c>
       <c r="B22" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C22" s="5" t="n">
         <v>1</v>
       </c>
+      <c r="C22" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>V2</t>
+          <t>REMIS</t>
         </is>
       </c>
     </row>
@@ -791,15 +791,15 @@
           <t>False Positive</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n">
-        <v>6</v>
+      <c r="B23" s="4" t="n">
+        <v>7</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>7</v>
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>REMIS</t>
         </is>
       </c>
     </row>
@@ -965,14 +965,14 @@
         </is>
       </c>
       <c r="B34" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C34" s="5" t="n">
         <v>6</v>
       </c>
+      <c r="C34" s="4" t="n">
+        <v>6</v>
+      </c>
       <c r="D34" s="4" t="inlineStr">
         <is>
-          <t>V2</t>
+          <t>REMIS</t>
         </is>
       </c>
     </row>
@@ -983,7 +983,7 @@
         </is>
       </c>
       <c r="B35" s="4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C35" s="4" t="n">
         <v>6</v>
@@ -1030,10 +1030,10 @@
         </is>
       </c>
       <c r="B39" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39" s="4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D39" s="4" t="inlineStr">
         <is>
@@ -1048,10 +1048,10 @@
         </is>
       </c>
       <c r="B40" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C40" s="4" t="n">
         <v>9</v>
-      </c>
-      <c r="C40" s="4" t="n">
-        <v>7</v>
       </c>
       <c r="D40" s="4" t="inlineStr">
         <is>
@@ -1066,7 +1066,7 @@
         </is>
       </c>
       <c r="B41" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>2</v>
@@ -1085,12 +1085,12 @@
       </c>
       <c r="B42" s="4" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="C42" s="4" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>78%</t>
         </is>
       </c>
       <c r="D42" s="4" t="inlineStr">
@@ -1408,7 +1408,7 @@
       <c r="G2" s="4" t="inlineStr"/>
       <c r="H2" s="4" t="inlineStr">
         <is>
-          <t>Małgorzata</t>
+          <t>Malgorzata</t>
         </is>
       </c>
       <c r="I2" s="4" t="inlineStr">
@@ -1443,15 +1443,25 @@
       </c>
       <c r="O2" s="4" t="inlineStr">
         <is>
-          <t>NIE</t>
-        </is>
-      </c>
-      <c r="P2" s="4" t="inlineStr"/>
-      <c r="Q2" s="4" t="inlineStr"/>
+          <t>TAK</t>
+        </is>
+      </c>
+      <c r="P2" s="4" t="n">
+        <v>7.513640000413421e+17</v>
+      </c>
+      <c r="Q2" s="4" t="inlineStr">
+        <is>
+          <t>Malgorzata Owerko</t>
+        </is>
+      </c>
       <c r="R2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" s="4" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="S2" s="4" t="inlineStr">
+        <is>
+          <t>E+P+L+F</t>
+        </is>
+      </c>
       <c r="T2" s="4" t="inlineStr">
         <is>
           <t>TAK</t>
@@ -1472,15 +1482,15 @@
       </c>
       <c r="X2" s="4" t="inlineStr">
         <is>
-          <t>create_new</t>
+          <t>link_to_existing</t>
         </is>
       </c>
       <c r="Y2" s="4" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="Z2" s="4" t="inlineStr">
         <is>
-          <t>Gosia</t>
+          <t>Malgorzata</t>
         </is>
       </c>
       <c r="AA2" s="4" t="inlineStr">
@@ -1511,15 +1521,25 @@
       </c>
       <c r="AG2" s="4" t="inlineStr">
         <is>
-          <t>NIE</t>
-        </is>
-      </c>
-      <c r="AH2" s="4" t="inlineStr"/>
-      <c r="AI2" s="4" t="inlineStr"/>
+          <t>TAK</t>
+        </is>
+      </c>
+      <c r="AH2" s="4" t="n">
+        <v>7.513640000413421e+17</v>
+      </c>
+      <c r="AI2" s="4" t="inlineStr">
+        <is>
+          <t>Malgorzata Owerko</t>
+        </is>
+      </c>
       <c r="AJ2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="4" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="AK2" s="4" t="inlineStr">
+        <is>
+          <t>E+L+F</t>
+        </is>
+      </c>
       <c r="AL2" s="4" t="inlineStr">
         <is>
           <t>TAK</t>
@@ -1540,11 +1560,11 @@
       </c>
       <c r="AP2" s="4" t="inlineStr">
         <is>
-          <t>create_new</t>
+          <t>link_to_existing</t>
         </is>
       </c>
       <c r="AQ2" s="4" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AR2" s="4" t="inlineStr">
         <is>
@@ -1554,14 +1574,14 @@
       <c r="AS2" s="4" t="inlineStr"/>
       <c r="AT2" s="4" t="inlineStr"/>
       <c r="AU2" s="4" t="inlineStr"/>
-      <c r="AV2" s="5" t="inlineStr">
-        <is>
-          <t>TRUE_NEGATIVE</t>
-        </is>
-      </c>
-      <c r="AW2" s="5" t="inlineStr">
-        <is>
-          <t>TRUE_NEGATIVE</t>
+      <c r="AV2" s="6" t="inlineStr">
+        <is>
+          <t>FALSE_POSITIVE</t>
+        </is>
+      </c>
+      <c r="AW2" s="6" t="inlineStr">
+        <is>
+          <t>FALSE_POSITIVE</t>
         </is>
       </c>
       <c r="AX2" s="6" t="inlineStr">
@@ -1824,11 +1844,19 @@
           <t>+48 606 608 932</t>
         </is>
       </c>
-      <c r="L4" s="4" t="inlineStr"/>
-      <c r="M4" s="4" t="inlineStr"/>
+      <c r="L4" s="4" t="inlineStr">
+        <is>
+          <t>Sano - Med</t>
+        </is>
+      </c>
+      <c r="M4" s="4" t="inlineStr">
+        <is>
+          <t>682-156-00-39</t>
+        </is>
+      </c>
       <c r="N4" s="4" t="inlineStr">
         <is>
-          <t>NIE</t>
+          <t>TAK</t>
         </is>
       </c>
       <c r="O4" s="4" t="inlineStr">
@@ -1854,12 +1882,22 @@
       </c>
       <c r="T4" s="4" t="inlineStr">
         <is>
-          <t>NIE</t>
-        </is>
-      </c>
-      <c r="U4" s="4" t="inlineStr"/>
-      <c r="V4" s="4" t="inlineStr"/>
-      <c r="W4" s="4" t="inlineStr"/>
+          <t>TAK</t>
+        </is>
+      </c>
+      <c r="U4" s="4" t="n">
+        <v>7.51364000002273e+17</v>
+      </c>
+      <c r="V4" s="4" t="inlineStr">
+        <is>
+          <t>SANO - MED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+        </is>
+      </c>
+      <c r="W4" s="4" t="inlineStr">
+        <is>
+          <t>NIP (siedziba)</t>
+        </is>
+      </c>
       <c r="X4" s="4" t="inlineStr">
         <is>
           <t>link_to_existing</t>
@@ -1978,7 +2016,7 @@
       </c>
       <c r="AX4" s="6" t="inlineStr">
         <is>
-          <t>FALSE_NEGATIVE</t>
+          <t>FALSE_POSITIVE</t>
         </is>
       </c>
       <c r="AY4" s="6" t="inlineStr">
@@ -2073,11 +2111,11 @@
       <c r="W5" s="4" t="inlineStr"/>
       <c r="X5" s="4" t="inlineStr">
         <is>
-          <t>link_to_existing</t>
+          <t>review_required</t>
         </is>
       </c>
       <c r="Y5" s="4" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="Z5" s="4" t="inlineStr">
         <is>
@@ -2387,7 +2425,7 @@
       </c>
       <c r="H7" s="4" t="inlineStr">
         <is>
-          <t>Magda</t>
+          <t>Magdalena</t>
         </is>
       </c>
       <c r="I7" s="4" t="inlineStr">
@@ -2445,7 +2483,7 @@
       </c>
       <c r="Z7" s="4" t="inlineStr">
         <is>
-          <t>Magda</t>
+          <t>Magdalena</t>
         </is>
       </c>
       <c r="AA7" s="4" t="inlineStr">
@@ -2851,7 +2889,7 @@
         </is>
       </c>
       <c r="Y9" s="4" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="Z9" s="4" t="inlineStr">
         <is>
@@ -2921,7 +2959,7 @@
         </is>
       </c>
       <c r="AQ9" s="4" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AR9" s="4" t="inlineStr">
         <is>
@@ -3012,11 +3050,19 @@
           <t>+48 668 793 039</t>
         </is>
       </c>
-      <c r="L10" s="4" t="inlineStr"/>
-      <c r="M10" s="4" t="inlineStr"/>
+      <c r="L10" s="4" t="inlineStr">
+        <is>
+          <t>Klinika Pawlikowski</t>
+        </is>
+      </c>
+      <c r="M10" s="4" t="inlineStr">
+        <is>
+          <t>732-122-06-54</t>
+        </is>
+      </c>
       <c r="N10" s="4" t="inlineStr">
         <is>
-          <t>NIE</t>
+          <t>TAK</t>
         </is>
       </c>
       <c r="O10" s="4" t="inlineStr">
@@ -3055,7 +3101,7 @@
       </c>
       <c r="W10" s="4" t="inlineStr">
         <is>
-          <t>domena email</t>
+          <t>NIP (siedziba)</t>
         </is>
       </c>
       <c r="X10" s="4" t="inlineStr">
@@ -3232,7 +3278,11 @@
           <t>alojz1543@gmail.com</t>
         </is>
       </c>
-      <c r="K11" s="4" t="inlineStr"/>
+      <c r="K11" s="4" t="inlineStr">
+        <is>
+          <t>+44 7925 714020</t>
+        </is>
+      </c>
       <c r="L11" s="4" t="inlineStr">
         <is>
           <t>Bruk bed</t>
@@ -3601,11 +3651,11 @@
       <c r="W13" s="4" t="inlineStr"/>
       <c r="X13" s="4" t="inlineStr">
         <is>
-          <t>link_to_existing</t>
+          <t>review_required</t>
         </is>
       </c>
       <c r="Y13" s="4" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="Z13" s="4" t="inlineStr">
         <is>
@@ -3811,7 +3861,7 @@
       </c>
       <c r="AA14" s="4" t="inlineStr">
         <is>
-          <t>Dabrowski</t>
+          <t>Dąbrowski</t>
         </is>
       </c>
       <c r="AB14" s="4" t="inlineStr">
@@ -3837,15 +3887,25 @@
       </c>
       <c r="AG14" s="4" t="inlineStr">
         <is>
-          <t>NIE</t>
-        </is>
-      </c>
-      <c r="AH14" s="4" t="inlineStr"/>
-      <c r="AI14" s="4" t="inlineStr"/>
+          <t>TAK</t>
+        </is>
+      </c>
+      <c r="AH14" s="4" t="n">
+        <v>7.513640000023284e+17</v>
+      </c>
+      <c r="AI14" s="4" t="inlineStr">
+        <is>
+          <t>Michał Dąbrowski</t>
+        </is>
+      </c>
       <c r="AJ14" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK14" s="4" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="AK14" s="4" t="inlineStr">
+        <is>
+          <t>E+L+F</t>
+        </is>
+      </c>
       <c r="AL14" s="4" t="inlineStr">
         <is>
           <t>TAK</t>
@@ -3866,11 +3926,11 @@
       </c>
       <c r="AP14" s="4" t="inlineStr">
         <is>
-          <t>create_new</t>
+          <t>link_to_existing</t>
         </is>
       </c>
       <c r="AQ14" s="4" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AR14" s="4" t="inlineStr">
         <is>
@@ -3885,9 +3945,9 @@
           <t>FALSE_POSITIVE</t>
         </is>
       </c>
-      <c r="AW14" s="5" t="inlineStr">
-        <is>
-          <t>TRUE_NEGATIVE</t>
+      <c r="AW14" s="6" t="inlineStr">
+        <is>
+          <t>FALSE_POSITIVE</t>
         </is>
       </c>
       <c r="AX14" s="6" t="inlineStr">
@@ -4009,7 +4069,7 @@
       <c r="AC15" s="4" t="inlineStr"/>
       <c r="AD15" s="4" t="inlineStr">
         <is>
-          <t>HVD Holding</t>
+          <t>HVD</t>
         </is>
       </c>
       <c r="AE15" s="4" t="inlineStr">
@@ -4178,7 +4238,7 @@
         </is>
       </c>
       <c r="Y16" s="4" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="Z16" s="4" t="inlineStr">
         <is>
@@ -4248,7 +4308,7 @@
         </is>
       </c>
       <c r="AQ16" s="4" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AR16" s="4" t="inlineStr">
         <is>
@@ -4427,34 +4487,46 @@
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr"/>
-      <c r="D2" s="4" t="inlineStr"/>
-      <c r="E2" s="4" t="n">
-        <v/>
+      <c r="D2" s="4" t="n">
+        <v>7.513640000413421e+17</v>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>Malgorzata Owerko</t>
+        </is>
       </c>
       <c r="F2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4" t="n">
-        <v/>
-      </c>
-      <c r="H2" s="5" t="inlineStr">
-        <is>
-          <t>TRUE_NEGATIVE</t>
-        </is>
-      </c>
-      <c r="I2" s="4" t="inlineStr"/>
-      <c r="J2" s="4" t="n">
-        <v/>
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
+        <is>
+          <t>E+P+L+F</t>
+        </is>
+      </c>
+      <c r="H2" s="6" t="inlineStr">
+        <is>
+          <t>FALSE_POSITIVE</t>
+        </is>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>7.513640000413421e+17</v>
+      </c>
+      <c r="J2" s="4" t="inlineStr">
+        <is>
+          <t>Malgorzata Owerko</t>
+        </is>
       </c>
       <c r="K2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4" t="n">
-        <v/>
-      </c>
-      <c r="M2" s="5" t="inlineStr">
-        <is>
-          <t>TRUE_NEGATIVE</t>
+        <v>4</v>
+      </c>
+      <c r="L2" s="4" t="inlineStr">
+        <is>
+          <t>E+L+F</t>
+        </is>
+      </c>
+      <c r="M2" s="6" t="inlineStr">
+        <is>
+          <t>FALSE_POSITIVE</t>
         </is>
       </c>
       <c r="N2" s="4" t="inlineStr"/>
@@ -4637,13 +4709,17 @@
           <t>SANO - MED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
-      <c r="P4" s="4" t="inlineStr"/>
-      <c r="Q4" s="4" t="n">
-        <v/>
+      <c r="P4" s="4" t="n">
+        <v>7.51364000002273e+17</v>
+      </c>
+      <c r="Q4" s="4" t="inlineStr">
+        <is>
+          <t>SANO - MED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+        </is>
       </c>
       <c r="R4" s="6" t="inlineStr">
         <is>
-          <t>FALSE_NEGATIVE</t>
+          <t>FALSE_POSITIVE</t>
         </is>
       </c>
       <c r="S4" s="4" t="n">
@@ -5370,19 +5446,25 @@
           <t>FALSE_POSITIVE</t>
         </is>
       </c>
-      <c r="I14" s="4" t="inlineStr"/>
-      <c r="J14" s="4" t="n">
-        <v/>
+      <c r="I14" s="4" t="n">
+        <v>7.513640000023284e+17</v>
+      </c>
+      <c r="J14" s="4" t="inlineStr">
+        <is>
+          <t>Michał Dąbrowski</t>
+        </is>
       </c>
       <c r="K14" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" s="4" t="n">
-        <v/>
-      </c>
-      <c r="M14" s="5" t="inlineStr">
-        <is>
-          <t>TRUE_NEGATIVE</t>
+        <v>4</v>
+      </c>
+      <c r="L14" s="4" t="inlineStr">
+        <is>
+          <t>E+L+F</t>
+        </is>
+      </c>
+      <c r="M14" s="6" t="inlineStr">
+        <is>
+          <t>FALSE_POSITIVE</t>
         </is>
       </c>
       <c r="N14" s="4" t="inlineStr"/>
@@ -5579,7 +5661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5635,7 +5717,7 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
@@ -5643,14 +5725,18 @@
           <t>V1</t>
         </is>
       </c>
-      <c r="D2" s="4" t="inlineStr"/>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>NOWY</t>
+        </is>
+      </c>
       <c r="E2" s="4" t="inlineStr"/>
       <c r="F2" s="4" t="n">
-        <v>7.513640000023895e+17</v>
+        <v>7.513640000413421e+17</v>
       </c>
       <c r="G2" s="4" t="inlineStr">
         <is>
-          <t>GEDEON MEDICA SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Malgorzata Owerko</t>
         </is>
       </c>
       <c r="H2" s="6" t="inlineStr">
@@ -5665,7 +5751,7 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
@@ -5673,14 +5759,18 @@
           <t>V2</t>
         </is>
       </c>
-      <c r="D3" s="4" t="inlineStr"/>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>NOWY</t>
+        </is>
+      </c>
       <c r="E3" s="4" t="inlineStr"/>
       <c r="F3" s="4" t="n">
-        <v>7.513640000023895e+17</v>
+        <v>7.513640000413421e+17</v>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
-          <t>GEDEON MEDICA SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Malgorzata Owerko</t>
         </is>
       </c>
       <c r="H3" s="6" t="inlineStr">
@@ -5691,11 +5781,11 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
@@ -5703,22 +5793,14 @@
           <t>V1</t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>zcrm_751364000042205086</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>Weronika Kulik</t>
-        </is>
-      </c>
+      <c r="D4" s="4" t="inlineStr"/>
+      <c r="E4" s="4" t="inlineStr"/>
       <c r="F4" s="4" t="n">
-        <v>7.513640000422052e+17</v>
+        <v>7.513640000023895e+17</v>
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t>Weronika Kulik</t>
+          <t>GEDEON MEDICA SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="H4" s="6" t="inlineStr">
@@ -5729,11 +5811,11 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -5741,22 +5823,14 @@
           <t>V2</t>
         </is>
       </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>zcrm_751364000042205086</t>
-        </is>
-      </c>
-      <c r="E5" s="4" t="inlineStr">
-        <is>
-          <t>Weronika Kulik</t>
-        </is>
-      </c>
+      <c r="D5" s="4" t="inlineStr"/>
+      <c r="E5" s="4" t="inlineStr"/>
       <c r="F5" s="4" t="n">
-        <v>7.513640000422052e+17</v>
+        <v>7.513640000023895e+17</v>
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t>Weronika Kulik</t>
+          <t>GEDEON MEDICA SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="H5" s="6" t="inlineStr">
@@ -5771,7 +5845,7 @@
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -5781,21 +5855,25 @@
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000042205015</t>
+          <t>zcrm_751364000042205086</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>VIVENTI CLINIC SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="inlineStr"/>
-      <c r="G6" s="4" t="n">
-        <v/>
+          <t>Weronika Kulik</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>7.513640000422052e+17</v>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>Weronika Kulik</t>
+        </is>
       </c>
       <c r="H6" s="6" t="inlineStr">
         <is>
-          <t>FALSE_NEGATIVE</t>
+          <t>FALSE_POSITIVE</t>
         </is>
       </c>
     </row>
@@ -5805,7 +5883,7 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -5815,31 +5893,35 @@
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000042205015</t>
+          <t>zcrm_751364000042205086</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>VIVENTI CLINIC SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
-        </is>
-      </c>
-      <c r="F7" s="4" t="inlineStr"/>
-      <c r="G7" s="4" t="n">
-        <v/>
+          <t>Weronika Kulik</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>7.513640000422052e+17</v>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>Weronika Kulik</t>
+        </is>
       </c>
       <c r="H7" s="6" t="inlineStr">
         <is>
-          <t>FALSE_NEGATIVE</t>
+          <t>FALSE_POSITIVE</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C8" s="4" t="inlineStr">
@@ -5849,35 +5931,31 @@
       </c>
       <c r="D8" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000042575004</t>
+          <t>zcrm_751364000042205015</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>Grzegorz Wolak</t>
-        </is>
-      </c>
-      <c r="F8" s="4" t="n">
-        <v>7.513640000425751e+17</v>
-      </c>
-      <c r="G8" s="4" t="inlineStr">
-        <is>
-          <t>Grzegorz Wolak</t>
-        </is>
+          <t>VIVENTI CLINIC SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+        </is>
+      </c>
+      <c r="F8" s="4" t="inlineStr"/>
+      <c r="G8" s="4" t="n">
+        <v/>
       </c>
       <c r="H8" s="6" t="inlineStr">
         <is>
-          <t>FALSE_POSITIVE</t>
+          <t>FALSE_NEGATIVE</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
@@ -5887,25 +5965,21 @@
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000042575004</t>
+          <t>zcrm_751364000042205015</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
         <is>
-          <t>Grzegorz Wolak</t>
-        </is>
-      </c>
-      <c r="F9" s="4" t="n">
-        <v>7.513640000425751e+17</v>
-      </c>
-      <c r="G9" s="4" t="inlineStr">
-        <is>
-          <t>Grzegorz Wolak</t>
-        </is>
+          <t>VIVENTI CLINIC SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+        </is>
+      </c>
+      <c r="F9" s="4" t="inlineStr"/>
+      <c r="G9" s="4" t="n">
+        <v/>
       </c>
       <c r="H9" s="6" t="inlineStr">
         <is>
-          <t>FALSE_POSITIVE</t>
+          <t>FALSE_NEGATIVE</t>
         </is>
       </c>
     </row>
@@ -5915,7 +5989,7 @@
       </c>
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C10" s="4" t="inlineStr">
@@ -5925,21 +5999,25 @@
       </c>
       <c r="D10" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000002273003</t>
+          <t>zcrm_751364000042575004</t>
         </is>
       </c>
       <c r="E10" s="4" t="inlineStr">
         <is>
-          <t>SANO - MED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
-        </is>
-      </c>
-      <c r="F10" s="4" t="inlineStr"/>
-      <c r="G10" s="4" t="n">
-        <v/>
+          <t>Grzegorz Wolak</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>7.513640000425751e+17</v>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>Grzegorz Wolak</t>
+        </is>
       </c>
       <c r="H10" s="6" t="inlineStr">
         <is>
-          <t>FALSE_NEGATIVE</t>
+          <t>FALSE_POSITIVE</t>
         </is>
       </c>
     </row>
@@ -5949,7 +6027,7 @@
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr">
@@ -5959,20 +6037,20 @@
       </c>
       <c r="D11" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000002273003</t>
+          <t>zcrm_751364000042575004</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>SANO - MED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Grzegorz Wolak</t>
         </is>
       </c>
       <c r="F11" s="4" t="n">
-        <v>7.51364000002273e+17</v>
+        <v>7.513640000425751e+17</v>
       </c>
       <c r="G11" s="4" t="inlineStr">
         <is>
-          <t>SANO - MED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Grzegorz Wolak</t>
         </is>
       </c>
       <c r="H11" s="6" t="inlineStr">
@@ -5983,11 +6061,11 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C12" s="4" t="inlineStr">
@@ -5997,20 +6075,20 @@
       </c>
       <c r="D12" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000042738002</t>
+          <t>zcrm_751364000002273003</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr">
         <is>
-          <t>Waldemar Kornacki Waldemar Kornacki</t>
+          <t>SANO - MED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="F12" s="4" t="n">
-        <v>7.513640000427379e+17</v>
+        <v>7.51364000002273e+17</v>
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>Waldemar Kornacki</t>
+          <t>SANO - MED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="H12" s="6" t="inlineStr">
@@ -6021,11 +6099,11 @@
     </row>
     <row r="13">
       <c r="A13" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr">
@@ -6035,20 +6113,20 @@
       </c>
       <c r="D13" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000042738002</t>
+          <t>zcrm_751364000002273003</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
         <is>
-          <t>Waldemar Kornacki Waldemar Kornacki</t>
+          <t>SANO - MED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="F13" s="4" t="n">
-        <v>7.513640000427379e+17</v>
+        <v>7.51364000002273e+17</v>
       </c>
       <c r="G13" s="4" t="inlineStr">
         <is>
-          <t>Waldemar Kornacki</t>
+          <t>SANO - MED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="H13" s="6" t="inlineStr">
@@ -6059,7 +6137,7 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B14" s="4" t="inlineStr">
         <is>
@@ -6073,20 +6151,20 @@
       </c>
       <c r="D14" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000043588184</t>
+          <t>zcrm_751364000042738002</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
         <is>
-          <t>Sylwia Dziurda</t>
+          <t>Waldemar Kornacki Waldemar Kornacki</t>
         </is>
       </c>
       <c r="F14" s="4" t="n">
-        <v>7.513640000435881e+17</v>
+        <v>7.513640000427379e+17</v>
       </c>
       <c r="G14" s="4" t="inlineStr">
         <is>
-          <t>Sylwia Dziurda</t>
+          <t>Waldemar Kornacki</t>
         </is>
       </c>
       <c r="H14" s="6" t="inlineStr">
@@ -6097,7 +6175,7 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
@@ -6111,20 +6189,20 @@
       </c>
       <c r="D15" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000043588184</t>
+          <t>zcrm_751364000042738002</t>
         </is>
       </c>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>Sylwia Dziurda</t>
+          <t>Waldemar Kornacki Waldemar Kornacki</t>
         </is>
       </c>
       <c r="F15" s="4" t="n">
-        <v>7.513640000435881e+17</v>
+        <v>7.513640000427379e+17</v>
       </c>
       <c r="G15" s="4" t="inlineStr">
         <is>
-          <t>Sylwia Dziurda</t>
+          <t>Waldemar Kornacki</t>
         </is>
       </c>
       <c r="H15" s="6" t="inlineStr">
@@ -6139,7 +6217,7 @@
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C16" s="4" t="inlineStr">
@@ -6149,20 +6227,20 @@
       </c>
       <c r="D16" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000002312084</t>
+          <t>zcrm_751364000043588184</t>
         </is>
       </c>
       <c r="E16" s="4" t="inlineStr">
         <is>
-          <t>MEDESTETIS DR KUSCHILL I DR GRODECKA</t>
+          <t>Sylwia Dziurda</t>
         </is>
       </c>
       <c r="F16" s="4" t="n">
-        <v>7.513640000022746e+17</v>
+        <v>7.513640000435881e+17</v>
       </c>
       <c r="G16" s="4" t="inlineStr">
         <is>
-          <t>POLSKA GRUPA ESTETYCZNA SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Sylwia Dziurda</t>
         </is>
       </c>
       <c r="H16" s="6" t="inlineStr">
@@ -6177,7 +6255,7 @@
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr">
@@ -6187,20 +6265,20 @@
       </c>
       <c r="D17" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000002312084</t>
+          <t>zcrm_751364000043588184</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>MEDESTETIS DR KUSCHILL I DR GRODECKA</t>
+          <t>Sylwia Dziurda</t>
         </is>
       </c>
       <c r="F17" s="4" t="n">
-        <v>7.513640000022746e+17</v>
+        <v>7.513640000435881e+17</v>
       </c>
       <c r="G17" s="4" t="inlineStr">
         <is>
-          <t>POLSKA GRUPA ESTETYCZNA SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Sylwia Dziurda</t>
         </is>
       </c>
       <c r="H17" s="6" t="inlineStr">
@@ -6211,11 +6289,11 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C18" s="4" t="inlineStr">
@@ -6225,20 +6303,20 @@
       </c>
       <c r="D18" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000043674001</t>
+          <t>zcrm_751364000002312084</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
         <is>
-          <t>Monika Janas</t>
+          <t>MEDESTETIS DR KUSCHILL I DR GRODECKA</t>
         </is>
       </c>
       <c r="F18" s="4" t="n">
-        <v>7.513640000436739e+17</v>
+        <v>7.513640000022746e+17</v>
       </c>
       <c r="G18" s="4" t="inlineStr">
         <is>
-          <t>Monika Janas</t>
+          <t>POLSKA GRUPA ESTETYCZNA SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="H18" s="6" t="inlineStr">
@@ -6249,11 +6327,11 @@
     </row>
     <row r="19">
       <c r="A19" s="4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
@@ -6263,20 +6341,20 @@
       </c>
       <c r="D19" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000043674001</t>
+          <t>zcrm_751364000002312084</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr">
         <is>
-          <t>Monika Janas</t>
+          <t>MEDESTETIS DR KUSCHILL I DR GRODECKA</t>
         </is>
       </c>
       <c r="F19" s="4" t="n">
-        <v>7.513640000436739e+17</v>
+        <v>7.513640000022746e+17</v>
       </c>
       <c r="G19" s="4" t="inlineStr">
         <is>
-          <t>Monika Janas</t>
+          <t>POLSKA GRUPA ESTETYCZNA SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="H19" s="6" t="inlineStr">
@@ -6291,7 +6369,7 @@
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
@@ -6301,20 +6379,20 @@
       </c>
       <c r="D20" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000002280588</t>
+          <t>zcrm_751364000043674001</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr">
         <is>
-          <t>GRUPA MEDYCZNA VERTIMED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Monika Janas</t>
         </is>
       </c>
       <c r="F20" s="4" t="n">
-        <v>7.513640000022807e+17</v>
+        <v>7.513640000436739e+17</v>
       </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>GRUPA MEDYCZNA VERTIMED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Monika Janas</t>
         </is>
       </c>
       <c r="H20" s="6" t="inlineStr">
@@ -6329,7 +6407,7 @@
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
@@ -6339,20 +6417,20 @@
       </c>
       <c r="D21" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000002280588</t>
+          <t>zcrm_751364000043674001</t>
         </is>
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>GRUPA MEDYCZNA VERTIMED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Monika Janas</t>
         </is>
       </c>
       <c r="F21" s="4" t="n">
-        <v>7.513640000022807e+17</v>
+        <v>7.513640000436739e+17</v>
       </c>
       <c r="G21" s="4" t="inlineStr">
         <is>
-          <t>GRUPA MEDYCZNA VERTIMED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Monika Janas</t>
         </is>
       </c>
       <c r="H21" s="6" t="inlineStr">
@@ -6363,11 +6441,11 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
@@ -6377,20 +6455,20 @@
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000044508493</t>
+          <t>zcrm_751364000002280588</t>
         </is>
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>Bartosz Pawlikowski</t>
+          <t>GRUPA MEDYCZNA VERTIMED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="F22" s="4" t="n">
-        <v>7.513640000445087e+17</v>
+        <v>7.513640000022807e+17</v>
       </c>
       <c r="G22" s="4" t="inlineStr">
         <is>
-          <t>Bartosz Pawlikowski</t>
+          <t>GRUPA MEDYCZNA VERTIMED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="H22" s="6" t="inlineStr">
@@ -6401,11 +6479,11 @@
     </row>
     <row r="23">
       <c r="A23" s="4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
@@ -6415,20 +6493,20 @@
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000044508493</t>
+          <t>zcrm_751364000002280588</t>
         </is>
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
-          <t>Bartosz Pawlikowski</t>
+          <t>GRUPA MEDYCZNA VERTIMED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="F23" s="4" t="n">
-        <v>7.513640000445087e+17</v>
+        <v>7.513640000022807e+17</v>
       </c>
       <c r="G23" s="4" t="inlineStr">
         <is>
-          <t>Bartosz Pawlikowski</t>
+          <t>GRUPA MEDYCZNA VERTIMED SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="H23" s="6" t="inlineStr">
@@ -6443,7 +6521,7 @@
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C24" s="4" t="inlineStr">
@@ -6453,20 +6531,20 @@
       </c>
       <c r="D24" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000039032003</t>
+          <t>zcrm_751364000044508493</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
-          <t>MEDEVAC BARTOSZ PAWLIKOWSKI</t>
+          <t>Bartosz Pawlikowski</t>
         </is>
       </c>
       <c r="F24" s="4" t="n">
-        <v>7.513640000390321e+17</v>
+        <v>7.513640000445087e+17</v>
       </c>
       <c r="G24" s="4" t="inlineStr">
         <is>
-          <t>MEDEVAC BARTOSZ PAWLIKOWSKI</t>
+          <t>Bartosz Pawlikowski</t>
         </is>
       </c>
       <c r="H24" s="6" t="inlineStr">
@@ -6481,7 +6559,7 @@
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
@@ -6491,20 +6569,20 @@
       </c>
       <c r="D25" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000039032003</t>
+          <t>zcrm_751364000044508493</t>
         </is>
       </c>
       <c r="E25" s="4" t="inlineStr">
         <is>
-          <t>MEDEVAC BARTOSZ PAWLIKOWSKI</t>
+          <t>Bartosz Pawlikowski</t>
         </is>
       </c>
       <c r="F25" s="4" t="n">
-        <v>7.513640000390321e+17</v>
+        <v>7.513640000445087e+17</v>
       </c>
       <c r="G25" s="4" t="inlineStr">
         <is>
-          <t>MEDEVAC BARTOSZ PAWLIKOWSKI</t>
+          <t>Bartosz Pawlikowski</t>
         </is>
       </c>
       <c r="H25" s="6" t="inlineStr">
@@ -6515,11 +6593,11 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C26" s="4" t="inlineStr">
@@ -6529,16 +6607,20 @@
       </c>
       <c r="D26" s="4" t="inlineStr">
         <is>
-          <t>NOWY</t>
-        </is>
-      </c>
-      <c r="E26" s="4" t="inlineStr"/>
+          <t>zcrm_751364000039032003</t>
+        </is>
+      </c>
+      <c r="E26" s="4" t="inlineStr">
+        <is>
+          <t>MEDEVAC BARTOSZ PAWLIKOWSKI</t>
+        </is>
+      </c>
       <c r="F26" s="4" t="n">
-        <v>7.513640000023429e+17</v>
+        <v>7.513640000390321e+17</v>
       </c>
       <c r="G26" s="4" t="inlineStr">
         <is>
-          <t>Daniel Szymański</t>
+          <t>MEDEVAC BARTOSZ PAWLIKOWSKI</t>
         </is>
       </c>
       <c r="H26" s="6" t="inlineStr">
@@ -6549,30 +6631,34 @@
     </row>
     <row r="27">
       <c r="A27" s="4" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>V2</t>
         </is>
       </c>
       <c r="D27" s="4" t="inlineStr">
         <is>
-          <t>NOWY</t>
-        </is>
-      </c>
-      <c r="E27" s="4" t="inlineStr"/>
+          <t>zcrm_751364000039032003</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="inlineStr">
+        <is>
+          <t>MEDEVAC BARTOSZ PAWLIKOWSKI</t>
+        </is>
+      </c>
       <c r="F27" s="4" t="n">
-        <v>7.513640000023284e+17</v>
+        <v>7.513640000390321e+17</v>
       </c>
       <c r="G27" s="4" t="inlineStr">
         <is>
-          <t>Michał Dąbrowski</t>
+          <t>MEDEVAC BARTOSZ PAWLIKOWSKI</t>
         </is>
       </c>
       <c r="H27" s="6" t="inlineStr">
@@ -6583,11 +6669,11 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C28" s="4" t="inlineStr">
@@ -6595,14 +6681,18 @@
           <t>V1</t>
         </is>
       </c>
-      <c r="D28" s="4" t="inlineStr"/>
+      <c r="D28" s="4" t="inlineStr">
+        <is>
+          <t>NOWY</t>
+        </is>
+      </c>
       <c r="E28" s="4" t="inlineStr"/>
       <c r="F28" s="4" t="n">
-        <v>7.513640000022842e+17</v>
+        <v>7.513640000023429e+17</v>
       </c>
       <c r="G28" s="4" t="inlineStr">
         <is>
-          <t>BONUM ENTERPRISE SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Daniel Szymański</t>
         </is>
       </c>
       <c r="H28" s="6" t="inlineStr">
@@ -6617,22 +6707,26 @@
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>Account</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
         <is>
-          <t>V2</t>
-        </is>
-      </c>
-      <c r="D29" s="4" t="inlineStr"/>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="D29" s="4" t="inlineStr">
+        <is>
+          <t>NOWY</t>
+        </is>
+      </c>
       <c r="E29" s="4" t="inlineStr"/>
       <c r="F29" s="4" t="n">
-        <v>7.513640000022842e+17</v>
+        <v>7.513640000023284e+17</v>
       </c>
       <c r="G29" s="4" t="inlineStr">
         <is>
-          <t>BONUM ENTERPRISE SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Michał Dąbrowski</t>
         </is>
       </c>
       <c r="H29" s="6" t="inlineStr">
@@ -6643,7 +6737,7 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
@@ -6652,25 +6746,21 @@
       </c>
       <c r="C30" s="4" t="inlineStr">
         <is>
-          <t>V1</t>
+          <t>V2</t>
         </is>
       </c>
       <c r="D30" s="4" t="inlineStr">
         <is>
-          <t>zcrm_751364000045867011</t>
-        </is>
-      </c>
-      <c r="E30" s="4" t="inlineStr">
-        <is>
-          <t>Patryk Derkowski</t>
-        </is>
-      </c>
+          <t>NOWY</t>
+        </is>
+      </c>
+      <c r="E30" s="4" t="inlineStr"/>
       <c r="F30" s="4" t="n">
-        <v>7.51364000045867e+17</v>
+        <v>7.513640000023284e+17</v>
       </c>
       <c r="G30" s="4" t="inlineStr">
         <is>
-          <t>Patryk Derkowski</t>
+          <t>Michał Dąbrowski</t>
         </is>
       </c>
       <c r="H30" s="6" t="inlineStr">
@@ -6681,34 +6771,26 @@
     </row>
     <row r="31">
       <c r="A31" s="4" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Account</t>
         </is>
       </c>
       <c r="C31" s="4" t="inlineStr">
         <is>
-          <t>V2</t>
-        </is>
-      </c>
-      <c r="D31" s="4" t="inlineStr">
-        <is>
-          <t>zcrm_751364000045867011</t>
-        </is>
-      </c>
-      <c r="E31" s="4" t="inlineStr">
-        <is>
-          <t>Patryk Derkowski</t>
-        </is>
-      </c>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="D31" s="4" t="inlineStr"/>
+      <c r="E31" s="4" t="inlineStr"/>
       <c r="F31" s="4" t="n">
-        <v>7.51364000045867e+17</v>
+        <v>7.513640000022842e+17</v>
       </c>
       <c r="G31" s="4" t="inlineStr">
         <is>
-          <t>Patryk Derkowski</t>
+          <t>BONUM ENTERPRISE SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="H31" s="6" t="inlineStr">
@@ -6719,7 +6801,7 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B32" s="4" t="inlineStr">
         <is>
@@ -6728,25 +6810,17 @@
       </c>
       <c r="C32" s="4" t="inlineStr">
         <is>
-          <t>V1</t>
-        </is>
-      </c>
-      <c r="D32" s="4" t="inlineStr">
-        <is>
-          <t>zcrm_751364000010723654</t>
-        </is>
-      </c>
-      <c r="E32" s="4" t="inlineStr">
-        <is>
-          <t>DENTALSAND SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
-        </is>
-      </c>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="D32" s="4" t="inlineStr"/>
+      <c r="E32" s="4" t="inlineStr"/>
       <c r="F32" s="4" t="n">
-        <v>7.513640000107236e+17</v>
+        <v>7.513640000022842e+17</v>
       </c>
       <c r="G32" s="4" t="inlineStr">
         <is>
-          <t>DENTALSAND SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>BONUM ENTERPRISE SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
       <c r="H32" s="6" t="inlineStr">
@@ -6761,33 +6835,147 @@
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
+          <t>Contact</t>
+        </is>
+      </c>
+      <c r="C33" s="4" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="D33" s="4" t="inlineStr">
+        <is>
+          <t>zcrm_751364000045867011</t>
+        </is>
+      </c>
+      <c r="E33" s="4" t="inlineStr">
+        <is>
+          <t>Patryk Derkowski</t>
+        </is>
+      </c>
+      <c r="F33" s="4" t="n">
+        <v>7.51364000045867e+17</v>
+      </c>
+      <c r="G33" s="4" t="inlineStr">
+        <is>
+          <t>Patryk Derkowski</t>
+        </is>
+      </c>
+      <c r="H33" s="6" t="inlineStr">
+        <is>
+          <t>FALSE_POSITIVE</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B34" s="4" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+      <c r="C34" s="4" t="inlineStr">
+        <is>
+          <t>V2</t>
+        </is>
+      </c>
+      <c r="D34" s="4" t="inlineStr">
+        <is>
+          <t>zcrm_751364000045867011</t>
+        </is>
+      </c>
+      <c r="E34" s="4" t="inlineStr">
+        <is>
+          <t>Patryk Derkowski</t>
+        </is>
+      </c>
+      <c r="F34" s="4" t="n">
+        <v>7.51364000045867e+17</v>
+      </c>
+      <c r="G34" s="4" t="inlineStr">
+        <is>
+          <t>Patryk Derkowski</t>
+        </is>
+      </c>
+      <c r="H34" s="6" t="inlineStr">
+        <is>
+          <t>FALSE_POSITIVE</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
           <t>Account</t>
         </is>
       </c>
-      <c r="C33" s="4" t="inlineStr">
+      <c r="C35" s="4" t="inlineStr">
+        <is>
+          <t>V1</t>
+        </is>
+      </c>
+      <c r="D35" s="4" t="inlineStr">
+        <is>
+          <t>zcrm_751364000010723654</t>
+        </is>
+      </c>
+      <c r="E35" s="4" t="inlineStr">
+        <is>
+          <t>DENTALSAND SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+        </is>
+      </c>
+      <c r="F35" s="4" t="n">
+        <v>7.513640000107236e+17</v>
+      </c>
+      <c r="G35" s="4" t="inlineStr">
+        <is>
+          <t>DENTALSAND SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+        </is>
+      </c>
+      <c r="H35" s="6" t="inlineStr">
+        <is>
+          <t>FALSE_POSITIVE</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="B36" s="4" t="inlineStr">
+        <is>
+          <t>Account</t>
+        </is>
+      </c>
+      <c r="C36" s="4" t="inlineStr">
         <is>
           <t>V2</t>
         </is>
       </c>
-      <c r="D33" s="4" t="inlineStr">
+      <c r="D36" s="4" t="inlineStr">
         <is>
           <t>zcrm_751364000010723654</t>
         </is>
       </c>
-      <c r="E33" s="4" t="inlineStr">
+      <c r="E36" s="4" t="inlineStr">
         <is>
           <t>DENTALSAND SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
-      <c r="F33" s="4" t="n">
+      <c r="F36" s="4" t="n">
         <v>7.513640000107236e+17</v>
       </c>
-      <c r="G33" s="4" t="inlineStr">
+      <c r="G36" s="4" t="inlineStr">
         <is>
           <t>DENTALSAND SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
-      <c r="H33" s="6" t="inlineStr">
+      <c r="H36" s="6" t="inlineStr">
         <is>
           <t>FALSE_POSITIVE</t>
         </is>

</xml_diff>